<commit_message>
Add city of Shoreline to sourceline
</commit_message>
<xml_diff>
--- a/data/pipeline.xlsx
+++ b/data/pipeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cortblad/Desktop/Hot News work/Apt planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cortblad/Documents/GitHub/apt-planning/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836E3F1D-C2E6-A94F-8E06-46A53A9E1264}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDCCCCF-96AB-CE4D-8DFE-7B8A0C3D99BA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24420" windowHeight="23260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Area</t>
   </si>
@@ -145,16 +145,26 @@
   </si>
   <si>
     <t>construction</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -192,10 +202,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +492,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -653,8 +666,8 @@
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C16">
         <v>353</v>
@@ -904,5 +917,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>